<commit_message>
Update CSS styles in Solo Bowl for improved design consistency and responsiveness; change font to Poppins and adjust background gradients
</commit_message>
<xml_diff>
--- a/Solo Bowl/EH (Solo Bowl).xlsx
+++ b/Solo Bowl/EH (Solo Bowl).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSM Projects\Solo Bowl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C0BCDD-FF76-4A66-813F-B72F5411500D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E47F2F1-9924-4E15-B11D-49FB9691D5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,7 +398,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>